<commit_message>
fixed bug where open trades fail to close
</commit_message>
<xml_diff>
--- a/ConfluenceValues.xlsx
+++ b/ConfluenceValues.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\RedPanda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Dropbox\Crypto\Python\ConfluenceCortex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C3740D02-1DDD-4162-9CD9-5ABEC1046A8D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B2B35B65-EAE5-478E-AF9C-7B953EC03351}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20805" windowHeight="14685" xr2:uid="{11A5419D-2F66-4E93-9520-53378A4B1113}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>